<commit_message>
after time_line was successfuly changed into time_due...
</commit_message>
<xml_diff>
--- a/pickles/dbcopy_insert.xlsx
+++ b/pickles/dbcopy_insert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plr03474\NoOneDrive\Python\ArturWebApp\pickles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D25FBB6-1B32-49ED-9282-5ADDF41704EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5F4B6FA-14A7-4019-93F0-8D1F085B8019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="72">
   <si>
     <t>id</t>
   </si>
@@ -46,9 +46,6 @@
     <t>time_completion</t>
   </si>
   <si>
-    <t>time_line</t>
-  </si>
-  <si>
     <t>duration_plan</t>
   </si>
   <si>
@@ -61,18 +58,114 @@
     <t>order</t>
   </si>
   <si>
+    <t>show_menu</t>
+  </si>
+  <si>
     <t>id_strategy</t>
   </si>
   <si>
     <t>id_project</t>
   </si>
   <si>
+    <t>Data clean for Georgios</t>
+  </si>
+  <si>
     <t>Action</t>
   </si>
   <si>
+    <t>Continues</t>
+  </si>
+  <si>
+    <t>Start datacamp - ultimate goal is data scientist</t>
+  </si>
+  <si>
     <t>OneTime</t>
   </si>
   <si>
+    <t>Learn Javascript + react vue or agular</t>
+  </si>
+  <si>
+    <t>Learn pytest</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>BUG: task update +4h works for next 1h (when loading), so SelectField shows 'now'. ALL changed with move '&gt;' '&lt;' will not WORK!!</t>
+  </si>
+  <si>
+    <t>Solution: update function for choices to pick correct timeline</t>
+  </si>
+  <si>
+    <t>BUG Solution: update function for choices to pick correct timeline</t>
+  </si>
+  <si>
+    <t>Adding tasks on timeline button on each category</t>
+  </si>
+  <si>
+    <t>New timeline logic and function - one for all</t>
+  </si>
+  <si>
+    <t>Timeline bug - edit task would not work</t>
+  </si>
+  <si>
+    <t>Set venv for Georgios</t>
+  </si>
+  <si>
+    <t>Set venv for Anand</t>
+  </si>
+  <si>
+    <t>Make overview of what was delivered by Anand and put in folders</t>
+  </si>
+  <si>
+    <t>Aggregate and clean data</t>
+  </si>
+  <si>
+    <t>Tax NL</t>
+  </si>
+  <si>
+    <t>Apply to addidas</t>
+  </si>
+  <si>
+    <t>Start exercise. Stop cancer and heart attack.</t>
+  </si>
+  <si>
+    <t>Read book</t>
+  </si>
+  <si>
+    <t>Parcels for cooper cleaning</t>
+  </si>
+  <si>
+    <t>Add Menu filter by strategy, Projects, timeline (button groups)</t>
+  </si>
+  <si>
+    <t>Double tracking number issue</t>
+  </si>
+  <si>
+    <t>Summary graph</t>
+  </si>
+  <si>
+    <t>Add a copy task button</t>
+  </si>
+  <si>
+    <t>Change Frequency - Continous into every X days (to cover running every 2 days)</t>
+  </si>
+  <si>
+    <t>Deploy to python everywhere</t>
+  </si>
+  <si>
+    <t>Add alconsumption</t>
+  </si>
+  <si>
+    <t>Buy binnenband 26 1.75</t>
+  </si>
+  <si>
+    <t>Rapair bakfiest</t>
+  </si>
+  <si>
+    <t>iPlan Feature: plan hrs in month and let script propose when including postponements</t>
+  </si>
+  <si>
     <t>symbol</t>
   </si>
   <si>
@@ -118,7 +211,7 @@
     <t>General</t>
   </si>
   <si>
-    <t>#DCDCDC</t>
+    <t>#b1b4b5</t>
   </si>
   <si>
     <t>Untracked</t>
@@ -133,13 +226,19 @@
     <t>#82d7ff</t>
   </si>
   <si>
+    <t>India ND</t>
+  </si>
+  <si>
+    <t>#97e8a0</t>
+  </si>
+  <si>
     <t>version_num</t>
   </si>
   <si>
-    <t>db4e7b025e52</t>
-  </si>
-  <si>
-    <t>Check</t>
+    <t>e17d35e4019d</t>
+  </si>
+  <si>
+    <t>time_due</t>
   </si>
 </sst>
 </file>
@@ -506,15 +605,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,58 +636,1225 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2">
+        <v>43929.612627627313</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43935.766892356449</v>
+      </c>
+      <c r="H2" s="2">
+        <v>43935</v>
+      </c>
+      <c r="I2" s="2">
+        <v>25569.0625</v>
+      </c>
+      <c r="J2" s="2">
+        <v>25569.102777777782</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2">
+        <v>43929.894150115739</v>
+      </c>
+      <c r="H3" s="2">
+        <v>43941.999305555553</v>
+      </c>
+      <c r="I3" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J3" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L3">
+        <v>205</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2">
+        <v>43929.905651006942</v>
+      </c>
+      <c r="H4" s="2">
+        <v>44560.999305555553</v>
+      </c>
+      <c r="I4" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J4" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L4">
+        <v>715</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2">
+        <v>43930.396010185177</v>
+      </c>
+      <c r="H5" s="2">
+        <v>43952</v>
+      </c>
+      <c r="I5" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J5" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L5">
+        <v>614</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2">
+        <v>43931.435558657409</v>
+      </c>
+      <c r="H6" s="2">
+        <v>43941.389502314807</v>
+      </c>
+      <c r="I6" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J6" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L6">
+        <v>104</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2">
+        <v>43931.501387314813</v>
+      </c>
+      <c r="H7" s="2">
+        <v>43941.389606481483</v>
+      </c>
+      <c r="I7" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J7" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L7">
+        <v>106</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2">
+        <v>43931.502632951393</v>
+      </c>
+      <c r="G8" s="2">
+        <v>43938.504277177628</v>
+      </c>
+      <c r="H8" s="2">
+        <v>43938</v>
+      </c>
+      <c r="I8" s="2">
+        <v>25569.013888888891</v>
+      </c>
+      <c r="J8" s="2">
+        <v>25569.03504046419</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="2">
+        <v>43934.352580879633</v>
+      </c>
+      <c r="H9" s="2">
+        <v>43941.389456018522</v>
+      </c>
+      <c r="I9" s="2">
+        <v>25569.083333333328</v>
+      </c>
+      <c r="J9" s="2">
+        <v>25569.005684610769</v>
+      </c>
+      <c r="K9" s="2">
+        <v>43941.600318467572</v>
+      </c>
+      <c r="L9">
+        <v>102</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2">
+        <v>43934.354310173607</v>
+      </c>
+      <c r="H10" s="2">
+        <v>43941.389479166668</v>
+      </c>
+      <c r="I10" s="2">
+        <v>25569.041666666672</v>
+      </c>
+      <c r="J10" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L10">
+        <v>103</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="2">
+        <v>43935.283698439664</v>
+      </c>
+      <c r="G11" s="2">
+        <v>43935.68423278183</v>
+      </c>
+      <c r="H11" s="2">
+        <v>43935</v>
+      </c>
+      <c r="I11" s="2">
+        <v>25569.020833333328</v>
+      </c>
+      <c r="J11" s="2">
+        <v>25569.041253623029</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="2">
+        <v>43935.285558815172</v>
+      </c>
+      <c r="H12" s="2">
+        <v>43943</v>
+      </c>
+      <c r="I12" s="2">
+        <v>25569.020833333328</v>
+      </c>
+      <c r="J12" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L12">
+        <v>407</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="2">
+        <v>43935.286250228703</v>
+      </c>
+      <c r="H13" s="2">
+        <v>43943</v>
+      </c>
+      <c r="I13" s="2">
+        <v>25569.041666666672</v>
+      </c>
+      <c r="J13" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L13">
+        <v>408</v>
+      </c>
+      <c r="M13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="2">
+        <v>43935.289253890449</v>
+      </c>
+      <c r="H14" s="2">
+        <v>43943</v>
+      </c>
+      <c r="I14" s="2">
+        <v>25569.083333333328</v>
+      </c>
+      <c r="J14" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L14">
+        <v>409</v>
+      </c>
+      <c r="M14" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="2">
+        <v>43935.29684765741</v>
+      </c>
+      <c r="H15" s="2">
+        <v>43943</v>
+      </c>
+      <c r="I15" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J15" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L15">
+        <v>410</v>
+      </c>
+      <c r="M15" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="2">
+        <v>43935.297219557011</v>
+      </c>
+      <c r="G16" s="2">
+        <v>43935.867519493208</v>
+      </c>
+      <c r="H16" s="2">
+        <v>43935.833333333343</v>
+      </c>
+      <c r="I16" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J16" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L16">
+        <v>206</v>
+      </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="2">
+        <v>43935.298676194892</v>
+      </c>
+      <c r="G17" s="2">
+        <v>43941.377913282093</v>
+      </c>
+      <c r="H17" s="2">
+        <v>43938.833333333343</v>
+      </c>
+      <c r="I17" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J17" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
+      </c>
+      <c r="M17" t="b">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2">
+        <v>43935.426763447816</v>
+      </c>
+      <c r="G18" s="2">
+        <v>43936.603081444307</v>
+      </c>
+      <c r="H18" s="2">
+        <v>43936.832638888889</v>
+      </c>
+      <c r="I18" s="2">
+        <v>25569.020833333328</v>
+      </c>
+      <c r="J18" s="2">
+        <v>25569.0492125563</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18" t="b">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="2">
+        <v>43935.68355912697</v>
+      </c>
+      <c r="G19" s="2">
+        <v>43938.746700308831</v>
+      </c>
+      <c r="H19" s="2">
+        <v>43938</v>
+      </c>
+      <c r="I19" s="2">
+        <v>25569.0625</v>
+      </c>
+      <c r="J19" s="2">
+        <v>25569.070608583312</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="2">
+        <v>43936.367193499042</v>
+      </c>
+      <c r="H20" s="2">
+        <v>43941.832638888889</v>
+      </c>
+      <c r="I20" s="2">
+        <v>25569.083333333328</v>
+      </c>
+      <c r="J20" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L20">
+        <v>112</v>
+      </c>
+      <c r="M20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2">
+        <v>43936.519748284118</v>
+      </c>
+      <c r="G21" s="2">
+        <v>43937.46911462432</v>
+      </c>
+      <c r="H21" s="2">
+        <v>43937.406736111108</v>
+      </c>
+      <c r="I21" s="2">
+        <v>25569.020833333328</v>
+      </c>
+      <c r="J21" s="2">
+        <v>25569.01439187054</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="2">
+        <v>43937.385781476172</v>
+      </c>
+      <c r="G22" s="2">
+        <v>43938.576848711098</v>
+      </c>
+      <c r="H22" s="2">
+        <v>43938.406736111108</v>
+      </c>
+      <c r="I22" s="2">
+        <v>25569.020833333328</v>
+      </c>
+      <c r="J22" s="2">
+        <v>25569.024670814961</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22" t="b">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2">
-        <v>43934.438430533868</v>
-      </c>
-      <c r="H2" s="2">
-        <v>43934</v>
-      </c>
-      <c r="I2" s="2">
-        <v>25569</v>
-      </c>
-      <c r="J2" s="2">
-        <v>25569</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="2">
+        <v>43938.42027111417</v>
+      </c>
+      <c r="G23" s="2">
+        <v>43938.746680572607</v>
+      </c>
+      <c r="H23" s="2">
+        <v>43938</v>
+      </c>
+      <c r="I23" s="2">
+        <v>25569.041666666672</v>
+      </c>
+      <c r="J23" s="2">
+        <v>25569.069571631469</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="2">
+        <v>43938.430392831251</v>
+      </c>
+      <c r="H24" s="2">
+        <v>43941.832638888889</v>
+      </c>
+      <c r="I24" s="2">
+        <v>25569.083333333328</v>
+      </c>
+      <c r="J24" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L24">
+        <v>113</v>
+      </c>
+      <c r="M24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="2">
+        <v>43938.493515521033</v>
+      </c>
+      <c r="G25" s="2">
+        <v>43940.635662302222</v>
+      </c>
+      <c r="H25" s="2">
+        <v>43940</v>
+      </c>
+      <c r="I25" s="2">
+        <v>25569.020833333328</v>
+      </c>
+      <c r="J25" s="2">
+        <v>25569.039258754539</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25" t="b">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="2">
+        <v>43940.552329095881</v>
+      </c>
+      <c r="G26" s="2">
+        <v>43941.59180947682</v>
+      </c>
+      <c r="H26" s="2">
+        <v>43941.542071759257</v>
+      </c>
+      <c r="I26" s="2">
+        <v>25569.020833333328</v>
+      </c>
+      <c r="J26" s="2">
+        <v>25569.02473680328</v>
+      </c>
+      <c r="L26">
+        <v>100</v>
+      </c>
+      <c r="M26" t="b">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>85</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="2">
+        <v>43941.289014953283</v>
+      </c>
+      <c r="H27" s="2">
+        <v>43941.832638888889</v>
+      </c>
+      <c r="I27" s="2">
+        <v>25569.041666666672</v>
+      </c>
+      <c r="J27" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L27">
+        <v>111</v>
+      </c>
+      <c r="M27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="2">
+        <v>43941.2957295866</v>
+      </c>
+      <c r="H28" s="2">
+        <v>43941.832638888889</v>
+      </c>
+      <c r="I28" s="2">
+        <v>25569.041666666672</v>
+      </c>
+      <c r="J28" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L28">
+        <v>101</v>
+      </c>
+      <c r="M28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>87</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="2">
+        <v>43941.306077157657</v>
+      </c>
+      <c r="H29" s="2">
+        <v>43941.541666666657</v>
+      </c>
+      <c r="I29" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J29" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L29">
+        <v>116</v>
+      </c>
+      <c r="M29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="2">
+        <v>43941.307375732533</v>
+      </c>
+      <c r="H30" s="2">
+        <v>43941.833333333343</v>
+      </c>
+      <c r="I30" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J30" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>89</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="2">
+        <v>43941.456113393069</v>
+      </c>
+      <c r="H31" s="2">
+        <v>43941.666666666657</v>
+      </c>
+      <c r="I31" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J31" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31" t="b">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="2">
+        <v>43941.456768108692</v>
+      </c>
+      <c r="H32" s="2">
+        <v>43941.666666666657</v>
+      </c>
+      <c r="I32" s="2">
+        <v>25569.083333333328</v>
+      </c>
+      <c r="J32" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32" t="b">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="2">
+        <v>43941.491816810783</v>
+      </c>
+      <c r="H33" s="2">
+        <v>43952</v>
+      </c>
+      <c r="I33" s="2">
+        <v>25569</v>
+      </c>
+      <c r="J33" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>92</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="2">
+        <v>43941.508476305084</v>
+      </c>
+      <c r="H34" s="2">
+        <v>43942.542071759257</v>
+      </c>
+      <c r="I34" s="2">
+        <v>25569.020833333328</v>
+      </c>
+      <c r="J34" s="2">
+        <v>25569</v>
+      </c>
+      <c r="L34">
+        <v>100</v>
+      </c>
+      <c r="M34" t="b">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -598,7 +1864,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -612,16 +1878,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -638,19 +1904,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>43924.962984901329</v>
+        <v>43924.962984895843</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -658,22 +1924,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="F3">
         <v>4</v>
       </c>
       <c r="G3" s="2">
-        <v>43925.481845765709</v>
+        <v>43925.48184576389</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -681,19 +1947,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="2">
-        <v>43926.487764078702</v>
+        <v>43926.487764074067</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -701,22 +1967,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" s="2">
-        <v>43926.949720448669</v>
+        <v>43926.94972045139</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -724,19 +1990,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" s="2">
-        <v>43929.396777382419</v>
+        <v>43929.39677738426</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -744,22 +2010,42 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7" s="2">
-        <v>43929.423342977861</v>
+        <v>43929.423342974544</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>43935.370733865879</v>
+      </c>
+      <c r="I8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -801,12 +2087,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>